<commit_message>
z80: Added PDF versions of docs
Updated VGA timings to render better through Google docs
</commit_message>
<xml_diff>
--- a/docs/Spectrum-VGA-timings.xlsx
+++ b/docs/Spectrum-VGA-timings.xlsx
@@ -7,19 +7,18 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Graphical" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Graphical!$A$4:$L$16</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Vertical refresh:</t>
   </si>
@@ -118,6 +117,12 @@
   </si>
   <si>
     <t>Horizontal refresh:</t>
+  </si>
+  <si>
+    <t>Sinclair ZX Spectrum on FPGA</t>
+  </si>
+  <si>
+    <t>VGA timings</t>
   </si>
 </sst>
 </file>
@@ -191,12 +196,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -223,6 +222,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -520,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -581,10 +587,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,10 +594,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -608,23 +610,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -643,6 +642,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -983,9 +986,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A21:C26" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A21:C26"/>
-  <sortState ref="A24:C28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A11:C16" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A11:C16"/>
+  <sortState ref="A22:C26">
     <sortCondition ref="A23:A28"/>
   </sortState>
   <tableColumns count="3">
@@ -998,9 +1001,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A29:C34" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A29:C34"/>
-  <sortState ref="A32:C36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A19:C24" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A19:C24"/>
+  <sortState ref="A30:C34">
     <sortCondition ref="A31:A36"/>
   </sortState>
   <tableColumns count="3">
@@ -1013,8 +1016,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A15:C18" totalsRowShown="0">
-  <autoFilter ref="A15:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="A5:C8" totalsRowShown="0">
+  <autoFilter ref="A5:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Parameter" dataDxfId="1"/>
     <tableColumn id="2" name="Value" dataDxfId="0"/>
@@ -1311,9 +1314,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D1" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="1">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="1">
+        <f>H4*8</f>
+        <v>256</v>
+      </c>
+      <c r="I5" s="1">
+        <f>I4*8</f>
+        <v>192</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>96</v>
+      </c>
+      <c r="E7" s="5">
+        <v>48</v>
+      </c>
+      <c r="F7" s="40">
+        <v>640</v>
+      </c>
+      <c r="G7" s="41"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="29">
+        <f>D7</f>
+        <v>96</v>
+      </c>
+      <c r="E8" s="29">
+        <f>E7</f>
+        <v>48</v>
+      </c>
+      <c r="F8" s="5">
+        <f>(640-G8)/2</f>
+        <v>64</v>
+      </c>
+      <c r="G8" s="35">
+        <f>256*2</f>
+        <v>512</v>
+      </c>
+      <c r="H8" s="5">
+        <f>(640-G8)/2</f>
+        <v>64</v>
+      </c>
+      <c r="I8" s="29">
+        <f>I7</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="22">
+        <v>2</v>
+      </c>
+      <c r="C9" s="29">
+        <f>B9</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>33</v>
+      </c>
+      <c r="C10" s="29">
+        <f>B10</f>
+        <v>33</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="30">
+        <f>J9+C9</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="43">
+        <v>480</v>
+      </c>
+      <c r="C11" s="5">
+        <f>(480-C12)/2</f>
+        <v>48</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="30">
+        <f>J10+C10</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="36">
+        <f>192*2</f>
+        <v>384</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="30">
+        <f>J11+C11</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="45"/>
+      <c r="C13" s="5">
+        <f>(480-C12)/2</f>
+        <v>48</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="30">
+        <f>J12+C12</f>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>10</v>
+      </c>
+      <c r="C14" s="29">
+        <f>B14</f>
+        <v>10</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="30">
+        <f>J13+C13</f>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="30">
+        <v>0</v>
+      </c>
+      <c r="E15" s="30">
+        <f>D15+D8</f>
+        <v>96</v>
+      </c>
+      <c r="F15" s="30">
+        <f>E15+E8</f>
+        <v>144</v>
+      </c>
+      <c r="G15" s="30">
+        <f>F15+F8</f>
+        <v>208</v>
+      </c>
+      <c r="H15" s="30">
+        <f>G15+G8</f>
+        <v>720</v>
+      </c>
+      <c r="I15" s="30">
+        <f>H15+H8</f>
+        <v>784</v>
+      </c>
+      <c r="J15" s="31"/>
+      <c r="K15" s="34">
+        <f>SUM(B9:B14)</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J16" s="33">
+        <f>SUM(D7:I7)</f>
+        <v>800</v>
+      </c>
+      <c r="K16" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1321,16 +1615,9 @@
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1341,7 +1628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1357,457 +1644,210 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>31.46875</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>25.175000000000001</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="9">
         <v>96</v>
       </c>
-      <c r="H4" s="5">
+      <c r="C12" s="11">
+        <v>3.8133068520357001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="9">
         <v>48</v>
       </c>
-      <c r="I4" s="43">
+      <c r="C13" s="11">
+        <v>1.9066534260179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="9">
         <v>640</v>
       </c>
-      <c r="J4" s="44"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="5">
+      <c r="C14" s="11">
+        <v>25.422045680238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="9">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G5" s="31">
-        <f>G4</f>
-        <v>96</v>
-      </c>
-      <c r="H5" s="31">
-        <f>H4</f>
-        <v>48</v>
-      </c>
-      <c r="I5" s="5">
-        <f>(640-J5)/2</f>
-        <v>64</v>
-      </c>
-      <c r="J5" s="37">
-        <f>256*2</f>
-        <v>512</v>
-      </c>
-      <c r="K5" s="5">
-        <f>(640-J5)/2</f>
-        <v>64</v>
-      </c>
-      <c r="L5" s="31">
-        <f>L4</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="22">
+      <c r="C15" s="11">
+        <v>0.63555114200595997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="38">
+        <v>800</v>
+      </c>
+      <c r="C16" s="39">
+        <v>31.777557100298001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="31">
-        <f>E6</f>
-        <v>2</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="5">
+      <c r="C20" s="11">
+        <v>6.3555114200595994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="9">
         <v>33</v>
       </c>
-      <c r="F7" s="31">
-        <f>E7</f>
-        <v>33</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="32">
-        <f>M6+F6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="46">
+      <c r="C21" s="11">
+        <v>1.0486593843098</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="9">
         <v>480</v>
       </c>
-      <c r="F8" s="5">
-        <f>(480-F9)/2</f>
-        <v>48</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="32">
-        <f>M7+F7</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="47"/>
-      <c r="F9" s="38">
-        <f>192*2</f>
-        <v>384</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="32">
-        <f>M8+F8</f>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="48"/>
-      <c r="F10" s="5">
-        <f>(480-F9)/2</f>
-        <v>48</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="32">
-        <f>M9+F9</f>
-        <v>467</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="5">
+      <c r="C22" s="11">
+        <v>15.253227408142999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="9">
         <v>10</v>
       </c>
-      <c r="F11" s="31">
-        <f>E11</f>
-        <v>10</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="32">
-        <f>M10+F10</f>
-        <v>515</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="32">
-        <v>0</v>
-      </c>
-      <c r="H12" s="32">
-        <f>G12+G5</f>
-        <v>96</v>
-      </c>
-      <c r="I12" s="32">
-        <f>H12+H5</f>
-        <v>144</v>
-      </c>
-      <c r="J12" s="32">
-        <f>I12+I5</f>
-        <v>208</v>
-      </c>
-      <c r="K12" s="32">
-        <f>J12+J5</f>
-        <v>720</v>
-      </c>
-      <c r="L12" s="32">
-        <f>K12+K5</f>
-        <v>784</v>
-      </c>
-      <c r="M12" s="33"/>
-      <c r="N12" s="36">
-        <f>SUM(E6:E11)</f>
+      <c r="C23" s="11">
+        <v>0.31777557100297998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="38">
         <v>525</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M13" s="35">
-        <f>SUM(G4:L4)</f>
-        <v>800</v>
-      </c>
-      <c r="N13" s="34"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1">
-        <v>31.46875</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
-        <v>25.175000000000001</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="9">
-        <v>96</v>
-      </c>
-      <c r="C22" s="11">
-        <v>3.8133068520357001</v>
-      </c>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="9">
-        <v>48</v>
-      </c>
-      <c r="C23" s="11">
-        <v>1.9066534260179</v>
-      </c>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="9">
-        <v>640</v>
-      </c>
-      <c r="C24" s="11">
-        <v>25.422045680238</v>
-      </c>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="9">
-        <v>16</v>
-      </c>
-      <c r="C25" s="11">
-        <v>0.63555114200595997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="40">
-        <v>800</v>
-      </c>
-      <c r="C26" s="41">
-        <v>31.777557100298001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="9">
-        <v>2</v>
-      </c>
-      <c r="C30" s="11">
-        <v>6.3555114200595994E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="9">
-        <v>33</v>
-      </c>
-      <c r="C31" s="11">
-        <v>1.0486593843098</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="9">
-        <v>480</v>
-      </c>
-      <c r="C32" s="11">
-        <v>15.253227408142999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="9">
-        <v>10</v>
-      </c>
-      <c r="C33" s="11">
-        <v>0.31777557100297998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="40">
-        <v>525</v>
-      </c>
-      <c r="C34" s="41">
+      <c r="C24" s="39">
         <v>16.683217477656001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="E8:E10"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>